<commit_message>
Entered timlog information for Albert, Monday 8/9 to Fridat 12/9
</commit_message>
<xml_diff>
--- a/Documents/Timelogs/Timelog - Albert.xlsx
+++ b/Documents/Timelogs/Timelog - Albert.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Hours</t>
   </si>
@@ -31,13 +31,34 @@
   </si>
   <si>
     <t>Albert</t>
+  </si>
+  <si>
+    <t>Marti</t>
+  </si>
+  <si>
+    <t>Reading about both projects</t>
+  </si>
+  <si>
+    <t>Running the programs, analyzing architecture</t>
+  </si>
+  <si>
+    <t>Setting up a repository, explaining the team the workflow</t>
+  </si>
+  <si>
+    <t>Setting up the repository in teammates computers and teaching how to use git</t>
+  </si>
+  <si>
+    <t>Brainstorming about the changes I want to make in the architecture</t>
+  </si>
+  <si>
+    <t>118/9/14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -64,58 +85,54 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="26"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -353,58 +370,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -709,184 +735,216 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" customWidth="1"/>
+    <col min="3" max="3" width="58.83203125" customWidth="1"/>
     <col min="4" max="6" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="71.25" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
+      <c r="A1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" ht="24" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="17">
+        <v>41860</v>
+      </c>
+      <c r="B3" s="7">
+        <v>3</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="17">
+        <v>41891</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="17">
+        <v>41921</v>
+      </c>
+      <c r="B5" s="10">
+        <v>3</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="17">
+        <v>41982</v>
+      </c>
+      <c r="B7" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" ht="12" customHeight="1">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added timelog for Friday Sept 13th for Albert
</commit_message>
<xml_diff>
--- a/Documents/Timelogs/Timelog - Albert.xlsx
+++ b/Documents/Timelogs/Timelog - Albert.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Hours</t>
   </si>
@@ -51,7 +51,10 @@
     <t>Brainstorming about the changes I want to make in the architecture</t>
   </si>
   <si>
-    <t>118/9/14</t>
+    <t>13/9/14</t>
+  </si>
+  <si>
+    <t>Writing down the design and architecture of the software as well as exploring the Twitter API</t>
   </si>
 </sst>
 </file>
@@ -736,14 +739,14 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="58.83203125" customWidth="1"/>
+    <col min="3" max="3" width="70.1640625" customWidth="1"/>
     <col min="4" max="6" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -809,8 +812,8 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A6" s="17" t="s">
-        <v>10</v>
+      <c r="A6" s="17">
+        <v>41952</v>
       </c>
       <c r="B6" s="8">
         <v>2</v>
@@ -835,9 +838,15 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
+      <c r="A8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="10">
+        <v>5</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>11</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
     </row>

</xml_diff>